<commit_message>
Implementacion de servicios BACKEND , encomiendas, rutas y conductores
</commit_message>
<xml_diff>
--- a/jjlsapp-backend/Inventario API REST - JJLS BACKEND.xlsx
+++ b/jjlsapp-backend/Inventario API REST - JJLS BACKEND.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drive\SPRING FRAMEWORK\workspaces\workspace\jjlsapp-backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drive\SPRING FRAMEWORK\workspaces\workspace\jjlsapp-backend\jjlsapp-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>METODO</t>
   </si>
@@ -53,13 +53,49 @@
     <t>GET</t>
   </si>
   <si>
-    <t>http://161.35.62.203:8080/jjlsapp-backend/swagger-ui.html</t>
-  </si>
-  <si>
-    <t>http://161.35.62.203:8080/jjlsapp-backend/usuarios</t>
-  </si>
-  <si>
-    <t>http://161.35.62.203:8080/jjlsapp-backend/oauth/token</t>
+    <t>Servicio para registro de vehiculos</t>
+  </si>
+  <si>
+    <t>Servicio para registro de departamentos</t>
+  </si>
+  <si>
+    <t>Servicio para consulta de departamentos</t>
+  </si>
+  <si>
+    <t>Servicio para registro de conductores</t>
+  </si>
+  <si>
+    <t>Servicio para consulta de conductores</t>
+  </si>
+  <si>
+    <t>Servicio para registro de encomiendas</t>
+  </si>
+  <si>
+    <t>Servicio para registro de programacion de rutas</t>
+  </si>
+  <si>
+    <t>http://localhost:9090/swagger-ui.html</t>
+  </si>
+  <si>
+    <t>http://localhost:9090/usuarios</t>
+  </si>
+  <si>
+    <t>http://localhost:9090/oauth/token</t>
+  </si>
+  <si>
+    <t>http://localhost:9090/rutas</t>
+  </si>
+  <si>
+    <t>http://localhost:9090/vehiculos</t>
+  </si>
+  <si>
+    <t>http://localhost:9090/departamentos</t>
+  </si>
+  <si>
+    <t>http://localhost:9090/conductores</t>
+  </si>
+  <si>
+    <t>http://localhost:9090/encomiendas</t>
   </si>
 </sst>
 </file>
@@ -91,7 +127,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,6 +143,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -139,11 +181,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -152,6 +191,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -433,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C5"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,85 +491,132 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="B9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="A10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="A11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -535,8 +626,15 @@
     <hyperlink ref="B4" r:id="rId1"/>
     <hyperlink ref="B5" r:id="rId2"/>
     <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId4"/>
+    <hyperlink ref="B7" r:id="rId5"/>
+    <hyperlink ref="B9" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B10" r:id="rId8"/>
+    <hyperlink ref="B11" r:id="rId9"/>
+    <hyperlink ref="B12" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agregan servicios descarga excel, consulta rutas, inicio de sesion sin JWT
</commit_message>
<xml_diff>
--- a/jjlsapp-backend/Inventario API REST - JJLS BACKEND.xlsx
+++ b/jjlsapp-backend/Inventario API REST - JJLS BACKEND.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>METODO</t>
   </si>
@@ -96,6 +96,18 @@
   </si>
   <si>
     <t>http://localhost:9090/encomiendas</t>
+  </si>
+  <si>
+    <t>Logear usuario sin JWT</t>
+  </si>
+  <si>
+    <t>Obtener rutas disponibles</t>
+  </si>
+  <si>
+    <t>http://localhost:9090/rutas/reportes</t>
+  </si>
+  <si>
+    <t>Servicio que descarga excel con reporte total programados</t>
   </si>
 </sst>
 </file>
@@ -181,7 +193,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -191,11 +203,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -477,25 +491,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="57" customWidth="1"/>
-    <col min="3" max="3" width="42.85546875" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -575,47 +589,80 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="8" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -633,8 +680,11 @@
     <hyperlink ref="B10" r:id="rId8"/>
     <hyperlink ref="B11" r:id="rId9"/>
     <hyperlink ref="B12" r:id="rId10"/>
+    <hyperlink ref="B13" r:id="rId11"/>
+    <hyperlink ref="B14" r:id="rId12"/>
+    <hyperlink ref="B15" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>